<commit_message>
Updates to fO2 plots
</commit_message>
<xml_diff>
--- a/SWIR_input.xlsx
+++ b/SWIR_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="280" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Magmatic fO2 (1200 dC, 1 atm)</t>
   </si>
@@ -85,6 +85,18 @@
   <si>
     <t>MgO</t>
   </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>ol/opx?</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +105,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,6 +143,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -155,7 +176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -173,8 +194,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -194,8 +220,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -204,6 +235,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -212,7 +245,10 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -541,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -553,7 +589,7 @@
     <col min="2" max="2" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -566,8 +602,14 @@
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>-0.19668096615006014</v>
       </c>
@@ -580,8 +622,14 @@
       <c r="D2" s="10">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="14">
+        <v>-52.896000000000001</v>
+      </c>
+      <c r="F2" s="14">
+        <v>10.673999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>-3.6602370719476696E-2</v>
       </c>
@@ -594,8 +642,14 @@
       <c r="D3" s="10">
         <v>6.62</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="14">
+        <v>-52.896000000000001</v>
+      </c>
+      <c r="F3" s="14">
+        <v>10.673999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>8.895869425167291E-4</v>
       </c>
@@ -608,8 +662,14 @@
       <c r="D4" s="10">
         <v>6.38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="14">
+        <v>-52.896000000000001</v>
+      </c>
+      <c r="F4" s="14">
+        <v>10.673999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="4">
         <v>-5.3355689251386451E-2</v>
       </c>
@@ -622,8 +682,14 @@
       <c r="D5">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="15">
+        <v>-52.994</v>
+      </c>
+      <c r="F5" s="15">
+        <v>11.157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="4">
         <v>-0.18338258260368789</v>
       </c>
@@ -636,8 +702,14 @@
       <c r="D6">
         <v>8.17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="15">
+        <v>-52.994</v>
+      </c>
+      <c r="F6" s="15">
+        <v>11.157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="4">
         <v>-0.22927118249246803</v>
       </c>
@@ -650,8 +722,14 @@
       <c r="D7">
         <v>7.41</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="15">
+        <v>-52.994</v>
+      </c>
+      <c r="F7" s="15">
+        <v>11.157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="3">
         <v>5.3619543642074774E-2</v>
       </c>
@@ -664,8 +742,14 @@
       <c r="D8" s="10">
         <v>4.88</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="14">
+        <v>-52.817</v>
+      </c>
+      <c r="F8" s="14">
+        <v>11.387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>-0.26182262364745945</v>
       </c>
@@ -678,8 +762,14 @@
       <c r="D9">
         <v>7.31</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="15">
+        <v>-52.749000000000002</v>
+      </c>
+      <c r="F9" s="15">
+        <v>11.711</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="4">
         <v>-0.14568274320438945</v>
       </c>
@@ -692,8 +782,14 @@
       <c r="D10">
         <v>7.22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="15">
+        <v>-52.749000000000002</v>
+      </c>
+      <c r="F10" s="15">
+        <v>11.711</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="3">
         <v>-0.40686131539933257</v>
       </c>
@@ -706,8 +802,14 @@
       <c r="D11" s="10">
         <v>8.19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="14">
+        <v>-52.588999999999999</v>
+      </c>
+      <c r="F11" s="14">
+        <v>12.132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3">
         <v>-0.20288673562893322</v>
       </c>
@@ -720,8 +822,14 @@
       <c r="D12" s="10">
         <v>5.94</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="14">
+        <v>-52.588999999999999</v>
+      </c>
+      <c r="F12" s="14">
+        <v>12.132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="3">
         <v>-0.17922180505024166</v>
       </c>
@@ -734,8 +842,14 @@
       <c r="D13" s="10">
         <v>6.61</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="14">
+        <v>-52.588999999999999</v>
+      </c>
+      <c r="F13" s="14">
+        <v>12.132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="3">
         <v>-3.4591801016278012E-2</v>
       </c>
@@ -748,8 +862,14 @@
       <c r="D14" s="10">
         <v>6.92</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="14">
+        <v>-52.588999999999999</v>
+      </c>
+      <c r="F14" s="14">
+        <v>12.132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="4">
         <v>-0.36700978832512909</v>
       </c>
@@ -762,8 +882,14 @@
       <c r="D15">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="15">
+        <v>-52.56</v>
+      </c>
+      <c r="F15" s="15">
+        <v>12.798999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="4">
         <v>-0.14632555499637334</v>
       </c>
@@ -776,8 +902,14 @@
       <c r="D16">
         <v>7.52</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="15">
+        <v>-52.56</v>
+      </c>
+      <c r="F16" s="15">
+        <v>12.798999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>-0.68901886081710906</v>
       </c>
@@ -790,8 +922,14 @@
       <c r="D17">
         <v>9.6199999999999992</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="15">
+        <v>-52.56</v>
+      </c>
+      <c r="F17" s="15">
+        <v>12.798999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="4">
         <v>-0.26732177532332813</v>
       </c>
@@ -804,8 +942,14 @@
       <c r="D18">
         <v>7.54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="15">
+        <v>-52.56</v>
+      </c>
+      <c r="F18" s="15">
+        <v>12.798999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3">
         <v>-0.23354123711206576</v>
       </c>
@@ -818,8 +962,14 @@
       <c r="D19" s="10">
         <v>6.65</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="14">
+        <v>-52.475000000000001</v>
+      </c>
+      <c r="F19" s="14">
+        <v>13.144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3">
         <v>-0.23314961404650347</v>
       </c>
@@ -832,8 +982,14 @@
       <c r="D20" s="10">
         <v>6.33</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="14">
+        <v>-52.475000000000001</v>
+      </c>
+      <c r="F20" s="14">
+        <v>13.144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3">
         <v>-0.27046049792225091</v>
       </c>
@@ -846,8 +1002,14 @@
       <c r="D21" s="10">
         <v>6.52</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="14">
+        <v>-52.475000000000001</v>
+      </c>
+      <c r="F21" s="14">
+        <v>13.144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3">
         <v>-0.37806123406201486</v>
       </c>
@@ -860,8 +1022,14 @@
       <c r="D22" s="10">
         <v>6.28</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="14">
+        <v>-52.475000000000001</v>
+      </c>
+      <c r="F22" s="14">
+        <v>13.144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="4">
         <v>-0.13404547393531985</v>
       </c>
@@ -874,8 +1042,14 @@
       <c r="D23">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="15">
+        <v>-52.286000000000001</v>
+      </c>
+      <c r="F23" s="15">
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="3">
         <v>9.4082968693196989E-2</v>
       </c>
@@ -888,8 +1062,14 @@
       <c r="D24" s="10">
         <v>6.29</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="14">
+        <v>-52.18</v>
+      </c>
+      <c r="F24" s="14">
+        <v>14.34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="3">
         <v>0.20389697558555753</v>
       </c>
@@ -902,8 +1082,14 @@
       <c r="D25" s="10">
         <v>5.14</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="14">
+        <v>-52.18</v>
+      </c>
+      <c r="F25" s="14">
+        <v>14.34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="3">
         <v>-0.50459630924990861</v>
       </c>
@@ -916,8 +1102,14 @@
       <c r="D26" s="10">
         <v>7.36</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="14">
+        <v>-52.18</v>
+      </c>
+      <c r="F26" s="14">
+        <v>14.34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="4">
         <v>2.9323297416800287E-2</v>
       </c>
@@ -930,8 +1122,14 @@
       <c r="D27">
         <v>6.42</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="15">
+        <v>-52.26</v>
+      </c>
+      <c r="F27" s="15">
+        <v>14.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="4">
         <v>-0.38357800688558008</v>
       </c>
@@ -944,8 +1142,14 @@
       <c r="D28">
         <v>6.21</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="15">
+        <v>-52.26</v>
+      </c>
+      <c r="F28" s="15">
+        <v>14.59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="3">
         <v>-4.0566550758390107E-2</v>
       </c>
@@ -958,8 +1162,14 @@
       <c r="D29" s="10">
         <v>6.56</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="14">
+        <v>-52.24</v>
+      </c>
+      <c r="F29" s="14">
+        <v>14.78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="3">
         <v>-0.37429007643186374</v>
       </c>
@@ -972,8 +1182,14 @@
       <c r="D30" s="10">
         <v>6.58</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="14">
+        <v>-52.24</v>
+      </c>
+      <c r="F30" s="14">
+        <v>14.78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="3">
         <v>-0.10125268248244446</v>
       </c>
@@ -985,6 +1201,12 @@
       </c>
       <c r="D31" s="10">
         <v>6.46</v>
+      </c>
+      <c r="E31" s="14">
+        <v>-52.24</v>
+      </c>
+      <c r="F31" s="14">
+        <v>14.78</v>
       </c>
     </row>
   </sheetData>
@@ -2163,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2174,7 +2396,7 @@
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2193,8 +2415,17 @@
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5">
         <v>0.94327716158393038</v>
       </c>
@@ -2213,8 +2444,17 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>-52.993833333333335</v>
+      </c>
+      <c r="I2">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="5">
         <v>1.0337440532443622</v>
       </c>
@@ -2233,8 +2473,17 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>-52.99</v>
+      </c>
+      <c r="I3">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="6">
         <v>-1.2395615233198409</v>
       </c>
@@ -2253,8 +2502,17 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>-52.679000000000002</v>
+      </c>
+      <c r="I4">
+        <v>11.81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="6">
         <v>-0.50560648488703386</v>
       </c>
@@ -2273,8 +2531,17 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>-52.679000000000002</v>
+      </c>
+      <c r="I5">
+        <v>11.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="6">
         <v>1.0938924073553853</v>
       </c>
@@ -2293,8 +2560,17 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>-52.679000000000002</v>
+      </c>
+      <c r="I6">
+        <v>11.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="6">
         <v>0.12373724553990506</v>
       </c>
@@ -2313,8 +2589,17 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>-52.679000000000002</v>
+      </c>
+      <c r="I7">
+        <v>11.81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="6">
         <v>0.52276579042969473</v>
       </c>
@@ -2333,8 +2618,17 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>-52.679000000000002</v>
+      </c>
+      <c r="I8">
+        <v>11.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="5">
         <v>0.34793670032998492</v>
       </c>
@@ -2353,8 +2647,17 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>-52.720166666666664</v>
+      </c>
+      <c r="I9">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="5">
         <v>0.58035911156526332</v>
       </c>
@@ -2373,8 +2676,17 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>-52.720166666666664</v>
+      </c>
+      <c r="I10">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="5">
         <v>1.2939309206634437</v>
       </c>
@@ -2393,8 +2705,17 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>-52.720166666666664</v>
+      </c>
+      <c r="I11">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="5">
         <v>1.1634455175215077</v>
       </c>
@@ -2413,8 +2734,17 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>-52.720166666666664</v>
+      </c>
+      <c r="I12">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="6">
         <v>1.4357908121784018</v>
       </c>
@@ -2433,8 +2763,17 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>-52.645333333333333</v>
+      </c>
+      <c r="I13">
+        <v>12.526166666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="5">
         <v>0.18163148167539411</v>
       </c>
@@ -2453,8 +2792,17 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>-52.561500000000002</v>
+      </c>
+      <c r="I14">
+        <v>12.662166666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="7">
         <v>0.10468184159756433</v>
       </c>
@@ -2473,8 +2821,17 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>-52.561500000000002</v>
+      </c>
+      <c r="I15">
+        <v>12.662166666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="7">
         <v>0.74810111175072613</v>
       </c>
@@ -2493,8 +2850,17 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>-52.561500000000002</v>
+      </c>
+      <c r="I16">
+        <v>12.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="7">
         <v>1.2083415512668712</v>
       </c>
@@ -2513,8 +2879,17 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>-52.561500000000002</v>
+      </c>
+      <c r="I17">
+        <v>12.66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="7">
         <v>1.0105530410083574</v>
       </c>
@@ -2533,8 +2908,17 @@
       <c r="F18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>-52.561500000000002</v>
+      </c>
+      <c r="I18">
+        <v>12.66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="6">
         <v>0.4905334027321544</v>
       </c>
@@ -2553,8 +2937,17 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>-52.419499999999999</v>
+      </c>
+      <c r="I19">
+        <v>12.747999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="6">
         <v>1.2274402808177456</v>
       </c>
@@ -2573,8 +2966,17 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>-52.419499999999999</v>
+      </c>
+      <c r="I20">
+        <v>12.747999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="6">
         <v>0.17678097228280265</v>
       </c>
@@ -2593,8 +2995,17 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>-52.419499999999999</v>
+      </c>
+      <c r="I21">
+        <v>12.747999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="5">
         <v>0.90243028204142028</v>
       </c>
@@ -2613,8 +3024,17 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>-52.35</v>
+      </c>
+      <c r="I22">
+        <v>13.133333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="5">
         <v>0.29628006189715173</v>
       </c>
@@ -2633,8 +3053,17 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>-52.35</v>
+      </c>
+      <c r="I23">
+        <v>13.133333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="5">
         <v>0.81942681228897207</v>
       </c>
@@ -2653,8 +3082,17 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>-52.35</v>
+      </c>
+      <c r="I24">
+        <v>13.133333333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="6">
         <v>1.1133572377965848</v>
       </c>
@@ -2673,8 +3111,17 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>-52.474833333333336</v>
+      </c>
+      <c r="I25">
+        <v>13.14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="6">
         <v>1.3249840248360183</v>
       </c>
@@ -2693,8 +3140,17 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>-52.474833333333336</v>
+      </c>
+      <c r="I26">
+        <v>13.14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="6">
         <v>0.83424457410594677</v>
       </c>
@@ -2713,8 +3169,17 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>-52.474833333333336</v>
+      </c>
+      <c r="I27">
+        <v>13.14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="5">
         <v>1.0345766669105956</v>
       </c>
@@ -2733,8 +3198,17 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <v>-52.433</v>
+      </c>
+      <c r="I28">
+        <v>13.41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="5">
         <v>0.21771488161924779</v>
       </c>
@@ -2753,8 +3227,17 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>9</v>
+      </c>
+      <c r="H29">
+        <v>-52.433</v>
+      </c>
+      <c r="I29">
+        <v>13.41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="5">
         <v>0.79428502562812398</v>
       </c>
@@ -2773,8 +3256,17 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <v>-52.433</v>
+      </c>
+      <c r="I30">
+        <v>13.41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="5">
         <v>1.0249364666349674</v>
       </c>
@@ -2793,8 +3285,17 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>-52.433</v>
+      </c>
+      <c r="I31">
+        <v>13.41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="6">
         <v>-0.68260692518868282</v>
       </c>
@@ -2813,8 +3314,17 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>-52.369666666666667</v>
+      </c>
+      <c r="I32">
+        <v>13.51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="6">
         <v>-0.9777529409805048</v>
       </c>
@@ -2833,8 +3343,17 @@
       <c r="F33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>-52.369666666666667</v>
+      </c>
+      <c r="I33">
+        <v>13.51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="5">
         <v>1.3559829749719867</v>
       </c>
@@ -2853,8 +3372,17 @@
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>11</v>
+      </c>
+      <c r="H34">
+        <v>-52.156666666666666</v>
+      </c>
+      <c r="I34">
+        <v>13.73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="5">
         <v>1.5025721608970439</v>
       </c>
@@ -2873,8 +3401,17 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>11</v>
+      </c>
+      <c r="H35">
+        <v>-52.156666666666666</v>
+      </c>
+      <c r="I35">
+        <v>13.73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="7">
         <v>0.95366615277379019</v>
       </c>
@@ -2893,8 +3430,17 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>11</v>
+      </c>
+      <c r="H36">
+        <v>-52.156666666666666</v>
+      </c>
+      <c r="I36">
+        <v>13.73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="8">
         <v>0.54775620556947757</v>
       </c>
@@ -2913,8 +3459,17 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>-52.277500000000003</v>
+      </c>
+      <c r="I37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="8">
         <v>0.51531585975974359</v>
       </c>
@@ -2933,8 +3488,17 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <v>-52.277500000000003</v>
+      </c>
+      <c r="I38">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="6">
         <v>0.99725466324911061</v>
       </c>
@@ -2953,8 +3517,17 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>12</v>
+      </c>
+      <c r="H39">
+        <v>-52.277500000000003</v>
+      </c>
+      <c r="I39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="5">
         <v>0.60890014767099387</v>
       </c>
@@ -2973,8 +3546,17 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>13</v>
+      </c>
+      <c r="H40">
+        <v>-52.143333333333331</v>
+      </c>
+      <c r="I40">
+        <v>15.156499999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="5">
         <v>0.1587691341396269</v>
       </c>
@@ -2993,8 +3575,17 @@
       <c r="F41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>13</v>
+      </c>
+      <c r="H41">
+        <v>-52.143333333333331</v>
+      </c>
+      <c r="I41">
+        <v>15.156499999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="6">
         <v>0.23647052570773575</v>
       </c>
@@ -3012,6 +3603,15 @@
       </c>
       <c r="F42">
         <v>0</v>
+      </c>
+      <c r="G42">
+        <v>14</v>
+      </c>
+      <c r="H42">
+        <v>-52.25333333333333</v>
+      </c>
+      <c r="I42">
+        <v>15.2325</v>
       </c>
     </row>
   </sheetData>
@@ -3026,10 +3626,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3039,7 +3639,7 @@
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3049,8 +3649,11 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>-0.47</v>
       </c>
@@ -3060,8 +3663,11 @@
       <c r="C2" s="4">
         <v>0.33045751956258052</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>-0.89</v>
       </c>
@@ -3071,8 +3677,11 @@
       <c r="C3" s="4">
         <v>-9.3441117606547053E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>-0.38</v>
       </c>
@@ -3082,8 +3691,11 @@
       <c r="C4" s="4">
         <v>0.41104674721761114</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>-0.62</v>
       </c>
@@ -3093,8 +3705,11 @@
       <c r="C5" s="4">
         <v>9.0706754809035672E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>-0.7</v>
       </c>
@@ -3104,8 +3719,11 @@
       <c r="C6" s="4">
         <v>0.33260736343613573</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>-0.87</v>
       </c>
@@ -3115,8 +3733,11 @@
       <c r="C7" s="4">
         <v>-0.40170282588538342</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>-0.26</v>
       </c>
@@ -3126,8 +3747,11 @@
       <c r="C8" s="4">
         <v>0.33204387359380405</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>-2.3199999999999998</v>
       </c>
@@ -3137,8 +3761,11 @@
       <c r="C9" s="4">
         <v>-1.3864165786496141</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>-2.15</v>
       </c>
@@ -3148,8 +3775,11 @@
       <c r="C10" s="4">
         <v>-1.4310202649941175</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>-2.31</v>
       </c>
@@ -3159,8 +3789,11 @@
       <c r="C11" s="4">
         <v>-1.394030709979182</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>-1.67</v>
       </c>
@@ -3170,8 +3803,11 @@
       <c r="C12" s="4">
         <v>-0.93860875404856259</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>-1.03</v>
       </c>
@@ -3181,8 +3817,11 @@
       <c r="C13" s="4">
         <v>-0.22927695661043224</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>-0.56000000000000005</v>
       </c>
@@ -3192,8 +3831,11 @@
       <c r="C14" s="4">
         <v>0.35189973088698245</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>-0.23</v>
       </c>
@@ -3203,8 +3845,11 @@
       <c r="C15" s="4">
         <v>0.66412905932957145</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>-1.41</v>
       </c>
@@ -3214,8 +3859,11 @@
       <c r="C16" s="4">
         <v>-0.70460850738937353</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>-0.57999999999999996</v>
       </c>
@@ -3225,8 +3873,11 @@
       <c r="C17" s="4">
         <v>-0.12366963924389829</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>-0.83</v>
       </c>
@@ -3236,8 +3887,11 @@
       <c r="C18" s="4">
         <v>-0.82752836900428406</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>-1.56</v>
       </c>
@@ -3247,8 +3901,11 @@
       <c r="C19" s="4">
         <v>-1.1467631508101661</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>-0.76</v>
       </c>
@@ -3258,8 +3915,11 @@
       <c r="C20" s="4">
         <v>0.23168177037651461</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>0.03</v>
       </c>
@@ -3269,8 +3929,11 @@
       <c r="C21" s="4">
         <v>0.59456667726300338</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>0.37</v>
       </c>
@@ -3280,8 +3943,11 @@
       <c r="C22" s="4">
         <v>0.97085732201132302</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>-0.35</v>
       </c>
@@ -3291,8 +3957,11 @@
       <c r="C23" s="4">
         <v>0.3490329396632319</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>-0.68</v>
       </c>
@@ -3302,8 +3971,11 @@
       <c r="C24" s="4">
         <v>2.1081314017960651E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>-1.1100000000000001</v>
       </c>
@@ -3313,8 +3985,11 @@
       <c r="C25" s="4">
         <v>-0.38147576980966846</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>-0.61</v>
       </c>
@@ -3324,8 +3999,11 @@
       <c r="C26" s="4">
         <v>0.28862710098872313</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>-1.96</v>
       </c>
@@ -3335,8 +4013,11 @@
       <c r="C27" s="4">
         <v>0.24779961503969794</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>-0.36</v>
       </c>
@@ -3346,8 +4027,11 @@
       <c r="C28" s="4">
         <v>-9.0918485999115006E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>0.48</v>
       </c>
@@ -3357,8 +4041,11 @@
       <c r="C29" s="4">
         <v>1.0323652240076662</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>-0.96</v>
       </c>
@@ -3368,8 +4055,11 @@
       <c r="C30" s="4">
         <v>-0.23718054490700879</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>-0.56000000000000005</v>
       </c>
@@ -3379,8 +4069,11 @@
       <c r="C31" s="4">
         <v>0.16570822522318807</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>-0.43</v>
       </c>
@@ -3390,9 +4083,13 @@
       <c r="C32" s="4">
         <v>2.3109319713711329E-2</v>
       </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3403,10 +4100,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3415,7 +4112,7 @@
     <col min="2" max="2" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -3428,8 +4125,14 @@
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>-0.47</v>
       </c>
@@ -3442,8 +4145,14 @@
       <c r="D2">
         <v>-16.816666666666666</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.33045751956258052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>-0.89</v>
       </c>
@@ -3456,8 +4165,14 @@
       <c r="D3">
         <v>-16.816666666666666</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-9.3441117606547053E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>-0.38</v>
       </c>
@@ -3470,8 +4185,14 @@
       <c r="D4">
         <v>-16.816666666666666</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.41104674721761114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>-0.62</v>
       </c>
@@ -3484,8 +4205,14 @@
       <c r="D5">
         <v>-7.666666666666667</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>9.0706754809035672E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>-0.7</v>
       </c>
@@ -3498,8 +4225,14 @@
       <c r="D6">
         <v>-7.666666666666667</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.33260736343613573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>-0.87</v>
       </c>
@@ -3512,8 +4245,14 @@
       <c r="D7">
         <v>1.6166666666666667</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-0.40170282588538342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>-0.26</v>
       </c>
@@ -3526,8 +4265,14 @@
       <c r="D8">
         <v>1.6166666666666667</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.33204387359380405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>-2.3199999999999998</v>
       </c>
@@ -3540,8 +4285,14 @@
       <c r="D9">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>-1.3864165786496141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>-2.15</v>
       </c>
@@ -3554,8 +4305,14 @@
       <c r="D10">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>-1.4310202649941175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>-2.31</v>
       </c>
@@ -3568,8 +4325,14 @@
       <c r="D11">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-1.394030709979182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>-1.67</v>
       </c>
@@ -3582,8 +4345,14 @@
       <c r="D12">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>-0.93860875404856259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>-1.03</v>
       </c>
@@ -3596,8 +4365,14 @@
       <c r="D13">
         <v>32.333333333333336</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>-0.22927695661043224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>-0.56000000000000005</v>
       </c>
@@ -3610,8 +4385,14 @@
       <c r="D14">
         <v>32.333333333333336</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.35189973088698245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>-0.23</v>
       </c>
@@ -3624,8 +4405,14 @@
       <c r="D15">
         <v>32.333333333333336</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.66412905932957145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>-1.41</v>
       </c>
@@ -3638,8 +4425,14 @@
       <c r="D16">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>-0.70460850738937353</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>-0.57999999999999996</v>
       </c>
@@ -3652,8 +4445,14 @@
       <c r="D17">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-0.12366963924389829</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>-0.83</v>
       </c>
@@ -3666,8 +4465,14 @@
       <c r="D18">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-0.82752836900428406</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>-1.56</v>
       </c>
@@ -3680,8 +4485,14 @@
       <c r="D19">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>-1.1467631508101661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>-0.76</v>
       </c>
@@ -3694,8 +4505,14 @@
       <c r="D20" s="9">
         <v>13.133333333333333</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.23168177037651461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>0.03</v>
       </c>
@@ -3708,8 +4525,14 @@
       <c r="D21">
         <v>-17.583333333333332</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.59456667726300338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>0.37</v>
       </c>
@@ -3722,8 +4545,14 @@
       <c r="D22">
         <v>-17.583333333333332</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.97085732201132302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>-0.35</v>
       </c>
@@ -3736,8 +4565,14 @@
       <c r="D23">
         <v>-11.8</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.3490329396632319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>-0.68</v>
       </c>
@@ -3750,8 +4585,14 @@
       <c r="D24">
         <v>-11.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>2.1081314017960651E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>-1.1100000000000001</v>
       </c>
@@ -3764,8 +4605,14 @@
       <c r="D25">
         <v>-11.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>-0.38147576980966846</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>-0.61</v>
       </c>
@@ -3778,8 +4625,14 @@
       <c r="D26">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.28862710098872313</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>-1.96</v>
       </c>
@@ -3792,8 +4645,14 @@
       <c r="D27">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.24779961503969794</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>-0.36</v>
       </c>
@@ -3806,8 +4665,14 @@
       <c r="D28">
         <v>65.816666666666663</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>-9.0918485999115006E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>0.48</v>
       </c>
@@ -3820,8 +4685,14 @@
       <c r="D29">
         <v>65.816666666666663</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1.0323652240076662</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>-0.96</v>
       </c>
@@ -3834,8 +4705,14 @@
       <c r="D30">
         <v>67.63333333333334</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>-0.23718054490700879</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>-0.56000000000000005</v>
       </c>
@@ -3848,8 +4725,14 @@
       <c r="D31">
         <v>67.63333333333334</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.16570822522318807</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>-0.43</v>
       </c>
@@ -3861,6 +4744,12 @@
       </c>
       <c r="D32">
         <v>67.63333333333334</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>2.3109319713711329E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>